<commit_message>
Client/Documentatie: Added batching + update logboek
</commit_message>
<xml_diff>
--- a/Documentatie/Logboeken/logboek containing.xlsx
+++ b/Documentatie/Logboeken/logboek containing.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="31">
   <si>
     <t>donderdag</t>
   </si>
@@ -163,6 +163,19 @@
     <t>Controlpanel,
 nifty menu,
 container model,</t>
+  </si>
+  <si>
+    <t>Korte vergadering:
+Logboek,
+Junit,
+FPS improvements,
+documentatie,
+warnings in client,</t>
+  </si>
+  <si>
+    <t>Korte vergadering:
+Nieuwe models,
+FPS improvements,</t>
   </si>
 </sst>
 </file>
@@ -601,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,21 +867,29 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>41610</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="11"/>
+    </row>
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>41611</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="C23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3">

</xml_diff>